<commit_message>
Starting working on a JSON (I also considered YAML) as a input file for each dic analysis.
I started working on a skeleton and modified the existing py files with that in mind.

Removed **convert_image_times2meta_data.py** and moved the function into the package under **dic.misc**

In **post_1_obtain_dic_strain.py**:
- All references to file names and directories were replaced by constants.
- Commented out code that was not relevant anymore.

In **post_2_merge_dic_ut.py**:
- All references to file names and directories were replaced by constants.
- Moved all functions to the top of the file
- commented out code not relevant.
</commit_message>
<xml_diff>
--- a/examples/imada_ut/output/total_data.xlsx
+++ b/examples/imada_ut/output/total_data.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -476,16 +476,16 @@
         <v>-0.002</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.0002657939828733999</v>
+        <v>-0.0001492525234607414</v>
       </c>
       <c r="E2" t="n">
-        <v>0.0003130178889342233</v>
+        <v>0.0003751785476187274</v>
       </c>
       <c r="F2" t="n">
-        <v>-8.806067907093647e-05</v>
+        <v>1.141755862876664e-05</v>
       </c>
       <c r="G2" t="n">
-        <v>0.000417302751550076</v>
+        <v>0.000273440719640744</v>
       </c>
     </row>
     <row r="3">
@@ -499,16 +499,16 @@
         <v>-0.002</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.0003100840854887743</v>
+        <v>-0.0001668308307687119</v>
       </c>
       <c r="E3" t="n">
-        <v>0.000362327465806649</v>
+        <v>0.0004541564673688244</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.0001284591165246855</v>
+        <v>5.11270817048424e-06</v>
       </c>
       <c r="G3" t="n">
-        <v>0.0004734858795907806</v>
+        <v>0.0003084974955464617</v>
       </c>
     </row>
     <row r="4">
@@ -522,16 +522,16 @@
         <v>0.041</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.0003296132101004778</v>
+        <v>-0.000166455912194495</v>
       </c>
       <c r="E4" t="n">
-        <v>0.0005394961824474316</v>
+        <v>0.0003457538251463759</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.0003806976816222051</v>
+        <v>-6.8588160271084e-05</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0009109929106233887</v>
+        <v>0.0003480559893193233</v>
       </c>
     </row>
     <row r="5">
@@ -545,16 +545,16 @@
         <v>0.12</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.0005752085494977544</v>
+        <v>-0.0003074600772168026</v>
       </c>
       <c r="E5" t="n">
-        <v>0.0007471221178154823</v>
+        <v>0.0005690348437412497</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.0005008181753447369</v>
+        <v>-0.0001410375650077755</v>
       </c>
       <c r="G5" t="n">
-        <v>0.001101639606453899</v>
+        <v>0.0007434575854140146</v>
       </c>
     </row>
     <row r="6">
@@ -568,16 +568,16 @@
         <v>0.203</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.0008054462448945957</v>
+        <v>-0.0002561475708596361</v>
       </c>
       <c r="E6" t="n">
-        <v>0.0008029070767837563</v>
+        <v>0.000731213151734378</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.0003604541244715245</v>
+        <v>7.462942984879441e-05</v>
       </c>
       <c r="G6" t="n">
-        <v>0.001325560303312968</v>
+        <v>0.0008149183176421527</v>
       </c>
     </row>
     <row r="7">
@@ -591,16 +591,16 @@
         <v>0.284</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.001492809892765318</v>
+        <v>-0.0007952420083928882</v>
       </c>
       <c r="E7" t="n">
-        <v>0.001023413408367433</v>
+        <v>0.0007669327867518013</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.000914336452089514</v>
+        <v>-0.0001439901670627671</v>
       </c>
       <c r="G7" t="n">
-        <v>0.001219412744267363</v>
+        <v>0.0007813229011057326</v>
       </c>
     </row>
     <row r="8">
@@ -614,16 +614,16 @@
         <v>0.366</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.002228056120909695</v>
+        <v>-0.001558241706063425</v>
       </c>
       <c r="E8" t="n">
-        <v>0.0011585007217029</v>
+        <v>0.0009174982917444845</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.001045712528702509</v>
+        <v>-0.0006958245633135317</v>
       </c>
       <c r="G8" t="n">
-        <v>0.001338449431830761</v>
+        <v>0.0009113217646957393</v>
       </c>
     </row>
     <row r="9">
@@ -637,16 +637,16 @@
         <v>0.448</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.003048481743392365</v>
+        <v>-0.001791393246764375</v>
       </c>
       <c r="E9" t="n">
-        <v>0.001509474475987282</v>
+        <v>0.0009838532079763903</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.002168824196362787</v>
+        <v>-0.0006111432113413573</v>
       </c>
       <c r="G9" t="n">
-        <v>0.001614761598964712</v>
+        <v>0.00103479530973122</v>
       </c>
     </row>
     <row r="10">
@@ -660,16 +660,16 @@
         <v>0.528</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.00353737562069632</v>
+        <v>-0.002664423691037936</v>
       </c>
       <c r="E10" t="n">
-        <v>0.001698784685257534</v>
+        <v>0.00119686657028616</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.002517986091283558</v>
+        <v>-0.00102889703745616</v>
       </c>
       <c r="G10" t="n">
-        <v>0.001968949434587761</v>
+        <v>0.001342873853804123</v>
       </c>
     </row>
     <row r="11">
@@ -683,16 +683,16 @@
         <v>0.609</v>
       </c>
       <c r="D11" t="n">
-        <v>-0.003370769776488212</v>
+        <v>-0.002575505722096556</v>
       </c>
       <c r="E11" t="n">
-        <v>0.001727553501973235</v>
+        <v>0.00120327131143525</v>
       </c>
       <c r="F11" t="n">
-        <v>-0.003213529415707667</v>
+        <v>-0.001454539151820797</v>
       </c>
       <c r="G11" t="n">
-        <v>0.002281415679403974</v>
+        <v>0.001591426721660959</v>
       </c>
     </row>
     <row r="12">
@@ -706,16 +706,16 @@
         <v>0.6870000000000001</v>
       </c>
       <c r="D12" t="n">
-        <v>-0.002719888662161993</v>
+        <v>-0.002263199244714214</v>
       </c>
       <c r="E12" t="n">
-        <v>0.001667846321098422</v>
+        <v>0.001302874009659258</v>
       </c>
       <c r="F12" t="n">
-        <v>-0.003712567928768977</v>
+        <v>-0.001828465431017573</v>
       </c>
       <c r="G12" t="n">
-        <v>0.002550602632329364</v>
+        <v>0.0019822060379798</v>
       </c>
     </row>
     <row r="13">
@@ -729,16 +729,16 @@
         <v>0.767</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.002281540802528601</v>
+        <v>-0.001825817819275841</v>
       </c>
       <c r="E13" t="n">
-        <v>0.001776626488701972</v>
+        <v>0.001415300851235822</v>
       </c>
       <c r="F13" t="n">
-        <v>-0.003793235927964435</v>
+        <v>-0.001971014179297292</v>
       </c>
       <c r="G13" t="n">
-        <v>0.002658740959610483</v>
+        <v>0.002367338123781169</v>
       </c>
     </row>
     <row r="14">
@@ -752,16 +752,16 @@
         <v>0.847</v>
       </c>
       <c r="D14" t="n">
-        <v>-0.001633001844635816</v>
+        <v>-0.001360065506204139</v>
       </c>
       <c r="E14" t="n">
-        <v>0.001689922078745651</v>
+        <v>0.001567120414000109</v>
       </c>
       <c r="F14" t="n">
-        <v>-0.003867862349113748</v>
+        <v>-0.00228394356235211</v>
       </c>
       <c r="G14" t="n">
-        <v>0.002818331494036272</v>
+        <v>0.002326127562037571</v>
       </c>
     </row>
     <row r="15">
@@ -775,16 +775,16 @@
         <v>0.926</v>
       </c>
       <c r="D15" t="n">
-        <v>-0.00113315851467332</v>
+        <v>-0.0008553801134132314</v>
       </c>
       <c r="E15" t="n">
-        <v>0.002088260669051285</v>
+        <v>0.001785443922566691</v>
       </c>
       <c r="F15" t="n">
-        <v>-0.003966298665396465</v>
+        <v>-0.002193928673129744</v>
       </c>
       <c r="G15" t="n">
-        <v>0.002887651240557443</v>
+        <v>0.002395116494657849</v>
       </c>
     </row>
     <row r="16">
@@ -798,16 +798,16 @@
         <v>1.008</v>
       </c>
       <c r="D16" t="n">
-        <v>-0.0004726154485359196</v>
+        <v>-8.049112746943694e-05</v>
       </c>
       <c r="E16" t="n">
-        <v>0.002607674235860196</v>
+        <v>0.00199648529113505</v>
       </c>
       <c r="F16" t="n">
-        <v>-0.004587083307424033</v>
+        <v>-0.002492555658738326</v>
       </c>
       <c r="G16" t="n">
-        <v>0.002801799769293174</v>
+        <v>0.002468502493022762</v>
       </c>
     </row>
     <row r="17">
@@ -821,16 +821,16 @@
         <v>1.087</v>
       </c>
       <c r="D17" t="n">
-        <v>0.0006017012711195667</v>
+        <v>0.0007856861750867731</v>
       </c>
       <c r="E17" t="n">
-        <v>0.002481037911000983</v>
+        <v>0.002154709674748395</v>
       </c>
       <c r="F17" t="n">
-        <v>-0.005400367444607531</v>
+        <v>-0.002670363720407616</v>
       </c>
       <c r="G17" t="n">
-        <v>0.003140792028107974</v>
+        <v>0.002542907697115611</v>
       </c>
     </row>
     <row r="18">
@@ -844,16 +844,16 @@
         <v>1.168</v>
       </c>
       <c r="D18" t="n">
-        <v>0.001751488770671744</v>
+        <v>0.001785711237857091</v>
       </c>
       <c r="E18" t="n">
-        <v>0.002498695732825982</v>
+        <v>0.00219523467467847</v>
       </c>
       <c r="F18" t="n">
-        <v>-0.005873604070903485</v>
+        <v>-0.003115803640935884</v>
       </c>
       <c r="G18" t="n">
-        <v>0.003526002395484755</v>
+        <v>0.002854638991953727</v>
       </c>
     </row>
     <row r="19">
@@ -867,16 +867,16 @@
         <v>1.249</v>
       </c>
       <c r="D19" t="n">
-        <v>0.002611580024703437</v>
+        <v>0.002604104946770006</v>
       </c>
       <c r="E19" t="n">
-        <v>0.00270980820854354</v>
+        <v>0.002254303375282758</v>
       </c>
       <c r="F19" t="n">
-        <v>-0.005799812007302656</v>
+        <v>-0.0034945581415616</v>
       </c>
       <c r="G19" t="n">
-        <v>0.003606626799021927</v>
+        <v>0.00299955499848012</v>
       </c>
     </row>
     <row r="20">
@@ -890,16 +890,16 @@
         <v>1.327</v>
       </c>
       <c r="D20" t="n">
-        <v>0.003784162955153699</v>
+        <v>0.003641912638370943</v>
       </c>
       <c r="E20" t="n">
-        <v>0.002739861008519605</v>
+        <v>0.002356683441773457</v>
       </c>
       <c r="F20" t="n">
-        <v>-0.006239307181290238</v>
+        <v>-0.0035890269073665</v>
       </c>
       <c r="G20" t="n">
-        <v>0.003702591702922761</v>
+        <v>0.003034988549123087</v>
       </c>
     </row>
     <row r="21">
@@ -913,16 +913,16 @@
         <v>1.407</v>
       </c>
       <c r="D21" t="n">
-        <v>0.00513295604785681</v>
+        <v>0.004962029421347891</v>
       </c>
       <c r="E21" t="n">
-        <v>0.002796307275196887</v>
+        <v>0.002339141550601582</v>
       </c>
       <c r="F21" t="n">
-        <v>-0.006961274044606957</v>
+        <v>-0.003886691507338494</v>
       </c>
       <c r="G21" t="n">
-        <v>0.004354902672370579</v>
+        <v>0.003280546662306615</v>
       </c>
     </row>
     <row r="22">
@@ -936,16 +936,16 @@
         <v>1.486</v>
       </c>
       <c r="D22" t="n">
-        <v>0.00661347282223863</v>
+        <v>0.006286051510017006</v>
       </c>
       <c r="E22" t="n">
-        <v>0.002739170582257837</v>
+        <v>0.002213627971863412</v>
       </c>
       <c r="F22" t="n">
-        <v>-0.007381284662705893</v>
+        <v>-0.004388017628658354</v>
       </c>
       <c r="G22" t="n">
-        <v>0.004277504318267929</v>
+        <v>0.003486768592067418</v>
       </c>
     </row>
     <row r="23">
@@ -959,16 +959,16 @@
         <v>1.566</v>
       </c>
       <c r="D23" t="n">
-        <v>0.008171178751540791</v>
+        <v>0.007598237770134289</v>
       </c>
       <c r="E23" t="n">
-        <v>0.002678945109043438</v>
+        <v>0.002406186760932904</v>
       </c>
       <c r="F23" t="n">
-        <v>-0.008332379487858787</v>
+        <v>-0.004644362936433557</v>
       </c>
       <c r="G23" t="n">
-        <v>0.004873430952925086</v>
+        <v>0.003628978367280227</v>
       </c>
     </row>
     <row r="24">
@@ -982,16 +982,16 @@
         <v>1.648</v>
       </c>
       <c r="D24" t="n">
-        <v>0.01022888346361209</v>
+        <v>0.009378753763078958</v>
       </c>
       <c r="E24" t="n">
-        <v>0.002103108640869446</v>
+        <v>0.002329625667892026</v>
       </c>
       <c r="F24" t="n">
-        <v>-0.009285817165556759</v>
+        <v>-0.005220589466833935</v>
       </c>
       <c r="G24" t="n">
-        <v>0.005449322371273993</v>
+        <v>0.00399052899844319</v>
       </c>
     </row>
     <row r="25">
@@ -1005,16 +1005,16 @@
         <v>1.726</v>
       </c>
       <c r="D25" t="n">
-        <v>0.01312563484624355</v>
+        <v>0.01187340931849925</v>
       </c>
       <c r="E25" t="n">
-        <v>0.00186059168273446</v>
+        <v>0.002295769406557339</v>
       </c>
       <c r="F25" t="n">
-        <v>-0.01064737950335769</v>
+        <v>-0.005772762539291962</v>
       </c>
       <c r="G25" t="n">
-        <v>0.00622757608031186</v>
+        <v>0.004703942086372866</v>
       </c>
     </row>
     <row r="26">
@@ -1028,16 +1028,16 @@
         <v>1.807</v>
       </c>
       <c r="D26" t="n">
-        <v>0.01634422396984186</v>
+        <v>0.0145946123396631</v>
       </c>
       <c r="E26" t="n">
-        <v>0.003639624147076811</v>
+        <v>0.002738723076357088</v>
       </c>
       <c r="F26" t="n">
-        <v>-0.01099878389721502</v>
+        <v>-0.006018774357222043</v>
       </c>
       <c r="G26" t="n">
-        <v>0.006790749607484096</v>
+        <v>0.005179514946597535</v>
       </c>
     </row>
     <row r="27">
@@ -1051,16 +1051,16 @@
         <v>1.886</v>
       </c>
       <c r="D27" t="n">
-        <v>0.02090563428636244</v>
+        <v>0.01879891934765319</v>
       </c>
       <c r="E27" t="n">
-        <v>0.005923559242891592</v>
+        <v>0.005114848797747945</v>
       </c>
       <c r="F27" t="n">
-        <v>-0.01084821828376879</v>
+        <v>-0.006288805170874276</v>
       </c>
       <c r="G27" t="n">
-        <v>0.006785417974590684</v>
+        <v>0.005703291836366072</v>
       </c>
     </row>
     <row r="28">
@@ -1074,16 +1074,16 @@
         <v>1.968</v>
       </c>
       <c r="D28" t="n">
-        <v>0.02656140046631641</v>
+        <v>0.02414033151231108</v>
       </c>
       <c r="E28" t="n">
-        <v>0.007804772178838309</v>
+        <v>0.007194901754476809</v>
       </c>
       <c r="F28" t="n">
-        <v>-0.01064291885705861</v>
+        <v>-0.005596670694304766</v>
       </c>
       <c r="G28" t="n">
-        <v>0.006578481573990194</v>
+        <v>0.006082323021559932</v>
       </c>
     </row>
     <row r="29">
@@ -1097,16 +1097,16 @@
         <v>2.05</v>
       </c>
       <c r="D29" t="n">
-        <v>0.03273901639416022</v>
+        <v>0.03027572721016493</v>
       </c>
       <c r="E29" t="n">
-        <v>0.009103256382190989</v>
+        <v>0.008748941193638431</v>
       </c>
       <c r="F29" t="n">
-        <v>-0.01069262038915589</v>
+        <v>-0.005392758021319361</v>
       </c>
       <c r="G29" t="n">
-        <v>0.006630927840956296</v>
+        <v>0.006359293828373118</v>
       </c>
     </row>
     <row r="30">
@@ -1120,16 +1120,16 @@
         <v>2.13</v>
       </c>
       <c r="D30" t="n">
-        <v>0.03919133832729251</v>
+        <v>0.03658420802840052</v>
       </c>
       <c r="E30" t="n">
-        <v>0.01165615114615825</v>
+        <v>0.01014789249659725</v>
       </c>
       <c r="F30" t="n">
-        <v>-0.0107637340529299</v>
+        <v>-0.00512966737528577</v>
       </c>
       <c r="G30" t="n">
-        <v>0.006701985853085568</v>
+        <v>0.006760704648376354</v>
       </c>
     </row>
     <row r="31">
@@ -1143,16 +1143,16 @@
         <v>2.214</v>
       </c>
       <c r="D31" t="n">
-        <v>0.04964299464588354</v>
+        <v>0.04303901183756528</v>
       </c>
       <c r="E31" t="n">
-        <v>0.02670708827922073</v>
+        <v>0.01333370497188103</v>
       </c>
       <c r="F31" t="n">
-        <v>-0.02300215669942183</v>
+        <v>-0.005102946779880659</v>
       </c>
       <c r="G31" t="n">
-        <v>0.01663538226791039</v>
+        <v>0.006942177812202479</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Moved Dic functions inside the materials lab pkg. Updated history.md - The mechanism for the area of interest.   - when [(tl_X, tl_Y), (br_X, br_Y)] are used no need for selection   - markers are displayed - It is possible and reliable to use the argument in the init. - Move DIC-imada analysis and processing functions into the package.   - consider how to make agnostic the two parts. - moved **result.dic** file inside the output
</commit_message>
<xml_diff>
--- a/examples/imada_ut/output/total_data.xlsx
+++ b/examples/imada_ut/output/total_data.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>